<commit_message>
Aggiornato file EXCEL 30.05.2025
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#S2INFORMATICASRLXX/S2INFORMATICA/LABGUI/3.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#S2INFORMATICASRLXX/S2INFORMATICA/LABGUI/3.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="322">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -527,6 +527,9 @@
   <si>
     <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altro (specificare)</t>
   </si>
   <si>
     <t xml:space="preserve">Il codice fiscale e' solo maiuscolo</t>
@@ -1302,9 +1305,6 @@
   </si>
   <si>
     <t xml:space="preserve">L’applicativo effettua controlli preventivi sul dato inserito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Altro (specificare)</t>
   </si>
   <si>
     <t xml:space="preserve">TIPO DOCUMENTO</t>
@@ -3946,11 +3946,11 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="H53" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K49" activeCellId="0" sqref="K49"/>
+      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="bottomRight" activeCell="K53" activeCellId="0" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3963,11 +3963,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.77"/>
@@ -4697,7 +4697,9 @@
       <c r="K18" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="L18" s="42"/>
+      <c r="L18" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="M18" s="33" t="s">
         <v>56</v>
       </c>
@@ -4731,22 +4733,22 @@
         <v>48</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I19" s="32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J19" s="33" t="s">
         <v>55</v>
@@ -4790,22 +4792,22 @@
         <v>48</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F20" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I20" s="32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>55</v>
@@ -4849,22 +4851,22 @@
         <v>48</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I21" s="32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J21" s="33" t="s">
         <v>55</v>
@@ -4908,22 +4910,22 @@
         <v>48</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E22" s="38" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I22" s="32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J22" s="33" t="s">
         <v>55</v>
@@ -4967,22 +4969,22 @@
         <v>48</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I23" s="32" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J23" s="33" t="s">
         <v>55</v>
@@ -5026,22 +5028,22 @@
         <v>48</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I24" s="32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J24" s="33" t="s">
         <v>55</v>
@@ -5085,22 +5087,22 @@
         <v>48</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I25" s="32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J25" s="33" t="s">
         <v>55</v>
@@ -5144,22 +5146,22 @@
         <v>48</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H26" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I26" s="32" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J26" s="33" t="s">
         <v>55</v>
@@ -5203,22 +5205,22 @@
         <v>48</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H27" s="32" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I27" s="32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J27" s="33" t="s">
         <v>55</v>
@@ -5262,22 +5264,22 @@
         <v>48</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E28" s="38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F28" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H28" s="32" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I28" s="32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J28" s="33" t="s">
         <v>55</v>
@@ -5321,22 +5323,22 @@
         <v>48</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F29" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I29" s="32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>55</v>
@@ -5380,22 +5382,22 @@
         <v>48</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F30" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H30" s="32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I30" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J30" s="33" t="s">
         <v>55</v>
@@ -5439,22 +5441,22 @@
         <v>48</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F31" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H31" s="32" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I31" s="32" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J31" s="33" t="s">
         <v>55</v>
@@ -5498,22 +5500,22 @@
         <v>48</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F32" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H32" s="32" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I32" s="32" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J32" s="33" t="s">
         <v>55</v>
@@ -5557,22 +5559,22 @@
         <v>48</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F33" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H33" s="32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I33" s="32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J33" s="33" t="s">
         <v>55</v>
@@ -5596,7 +5598,7 @@
         <v>55</v>
       </c>
       <c r="S33" s="33" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T33" s="33"/>
       <c r="U33" s="34"/>
@@ -5616,22 +5618,22 @@
         <v>48</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E34" s="38" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F34" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H34" s="32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I34" s="32" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J34" s="33" t="s">
         <v>55</v>
@@ -5655,7 +5657,7 @@
         <v>55</v>
       </c>
       <c r="S34" s="33" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T34" s="33"/>
       <c r="U34" s="34"/>
@@ -5675,22 +5677,22 @@
         <v>48</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F35" s="30" t="s">
         <v>69</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H35" s="32" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I35" s="32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J35" s="33" t="s">
         <v>55</v>
@@ -5734,22 +5736,22 @@
         <v>48</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E36" s="48" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F36" s="49" t="s">
         <v>69</v>
       </c>
       <c r="G36" s="50" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H36" s="51" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I36" s="51" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J36" s="52" t="s">
         <v>55</v>
@@ -5775,25 +5777,25 @@
         <v>47</v>
       </c>
       <c r="C37" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E37" s="58" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F37" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G37" s="41" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H37" s="41" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I37" s="41" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J37" s="42" t="s">
         <v>55</v>
@@ -5826,25 +5828,25 @@
         <v>47</v>
       </c>
       <c r="C38" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D38" s="57" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E38" s="58" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F38" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H38" s="41" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I38" s="41" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J38" s="42" t="s">
         <v>55</v>
@@ -5877,25 +5879,25 @@
         <v>47</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D39" s="57" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E39" s="58" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F39" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H39" s="41" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I39" s="41" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J39" s="42" t="s">
         <v>55</v>
@@ -5928,25 +5930,25 @@
         <v>47</v>
       </c>
       <c r="C40" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D40" s="57" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F40" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G40" s="41" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H40" s="41" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I40" s="41" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J40" s="42" t="s">
         <v>55</v>
@@ -5979,25 +5981,25 @@
         <v>47</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D41" s="57" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E41" s="58" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F41" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G41" s="41" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H41" s="41" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I41" s="41" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J41" s="42" t="s">
         <v>55</v>
@@ -6030,22 +6032,22 @@
         <v>47</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D42" s="57" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E42" s="59" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F42" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G42" s="41" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H42" s="41" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I42" s="41" t="s">
         <v>54</v>
@@ -6074,7 +6076,7 @@
         <v>55</v>
       </c>
       <c r="S42" s="42" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="T42" s="42"/>
       <c r="U42" s="43"/>
@@ -6091,22 +6093,22 @@
         <v>47</v>
       </c>
       <c r="C43" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D43" s="57" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E43" s="59" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F43" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G43" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H43" s="41" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I43" s="41" t="s">
         <v>54</v>
@@ -6123,7 +6125,7 @@
         <v>55</v>
       </c>
       <c r="O43" s="42" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="P43" s="42" t="s">
         <v>55</v>
@@ -6135,7 +6137,7 @@
         <v>55</v>
       </c>
       <c r="S43" s="42" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="T43" s="42"/>
       <c r="U43" s="43"/>
@@ -6152,13 +6154,13 @@
         <v>47</v>
       </c>
       <c r="C44" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D44" s="57" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E44" s="58" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F44" s="39"/>
       <c r="G44" s="41"/>
@@ -6176,7 +6178,7 @@
         <v>55</v>
       </c>
       <c r="O44" s="42" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="P44" s="42" t="s">
         <v>55</v>
@@ -6188,7 +6190,7 @@
         <v>55</v>
       </c>
       <c r="S44" s="42" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="T44" s="42"/>
       <c r="U44" s="43"/>
@@ -6205,13 +6207,13 @@
         <v>47</v>
       </c>
       <c r="C45" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D45" s="57" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F45" s="39"/>
       <c r="G45" s="40"/>
@@ -6221,9 +6223,11 @@
         <v>56</v>
       </c>
       <c r="K45" s="42" t="s">
-        <v>230</v>
-      </c>
-      <c r="L45" s="42"/>
+        <v>96</v>
+      </c>
+      <c r="L45" s="42" t="s">
+        <v>231</v>
+      </c>
       <c r="M45" s="42"/>
       <c r="N45" s="42"/>
       <c r="O45" s="42"/>
@@ -6250,13 +6254,13 @@
         <v>47</v>
       </c>
       <c r="C46" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D46" s="57" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E46" s="58" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F46" s="39"/>
       <c r="G46" s="40"/>
@@ -6268,7 +6272,9 @@
       <c r="K46" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="L46" s="42"/>
+      <c r="L46" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="M46" s="33" t="s">
         <v>56</v>
       </c>
@@ -6299,13 +6305,13 @@
         <v>47</v>
       </c>
       <c r="C47" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D47" s="57" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E47" s="58" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F47" s="39"/>
       <c r="G47" s="40"/>
@@ -6315,9 +6321,11 @@
         <v>56</v>
       </c>
       <c r="K47" s="42" t="s">
-        <v>235</v>
-      </c>
-      <c r="L47" s="42"/>
+        <v>96</v>
+      </c>
+      <c r="L47" s="42" t="s">
+        <v>236</v>
+      </c>
       <c r="M47" s="42"/>
       <c r="N47" s="42"/>
       <c r="O47" s="42"/>
@@ -6344,13 +6352,13 @@
         <v>47</v>
       </c>
       <c r="C48" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D48" s="57" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E48" s="58" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F48" s="39"/>
       <c r="G48" s="40"/>
@@ -6360,9 +6368,11 @@
         <v>56</v>
       </c>
       <c r="K48" s="42" t="s">
-        <v>238</v>
-      </c>
-      <c r="L48" s="42"/>
+        <v>96</v>
+      </c>
+      <c r="L48" s="42" t="s">
+        <v>239</v>
+      </c>
       <c r="M48" s="42"/>
       <c r="N48" s="42"/>
       <c r="O48" s="42"/>
@@ -6389,13 +6399,13 @@
         <v>47</v>
       </c>
       <c r="C49" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D49" s="57" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E49" s="58" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F49" s="39"/>
       <c r="G49" s="40"/>
@@ -6405,9 +6415,11 @@
         <v>56</v>
       </c>
       <c r="K49" s="42" t="s">
-        <v>241</v>
-      </c>
-      <c r="L49" s="42"/>
+        <v>96</v>
+      </c>
+      <c r="L49" s="42" t="s">
+        <v>242</v>
+      </c>
       <c r="M49" s="42"/>
       <c r="N49" s="42"/>
       <c r="O49" s="42"/>
@@ -6434,13 +6446,13 @@
         <v>47</v>
       </c>
       <c r="C50" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D50" s="57" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E50" s="58" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F50" s="39"/>
       <c r="G50" s="40"/>
@@ -6450,9 +6462,11 @@
         <v>56</v>
       </c>
       <c r="K50" s="42" t="s">
-        <v>244</v>
-      </c>
-      <c r="L50" s="42"/>
+        <v>96</v>
+      </c>
+      <c r="L50" s="42" t="s">
+        <v>245</v>
+      </c>
       <c r="M50" s="42"/>
       <c r="N50" s="42"/>
       <c r="O50" s="42"/>
@@ -6479,13 +6493,13 @@
         <v>47</v>
       </c>
       <c r="C51" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D51" s="57" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E51" s="58" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F51" s="39"/>
       <c r="G51" s="40"/>
@@ -6495,9 +6509,11 @@
         <v>56</v>
       </c>
       <c r="K51" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="L51" s="42"/>
+        <v>96</v>
+      </c>
+      <c r="L51" s="42" t="s">
+        <v>248</v>
+      </c>
       <c r="M51" s="42"/>
       <c r="N51" s="42"/>
       <c r="O51" s="42"/>
@@ -6524,13 +6540,13 @@
         <v>47</v>
       </c>
       <c r="C52" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D52" s="57" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E52" s="58" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F52" s="39"/>
       <c r="G52" s="40"/>
@@ -6540,9 +6556,11 @@
         <v>56</v>
       </c>
       <c r="K52" s="42" t="s">
-        <v>250</v>
-      </c>
-      <c r="L52" s="42"/>
+        <v>96</v>
+      </c>
+      <c r="L52" s="42" t="s">
+        <v>251</v>
+      </c>
       <c r="M52" s="42"/>
       <c r="N52" s="42"/>
       <c r="O52" s="42"/>
@@ -6569,25 +6587,25 @@
         <v>47</v>
       </c>
       <c r="C53" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D53" s="57" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E53" s="58" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F53" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G53" s="40" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H53" s="41" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I53" s="41" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J53" s="42" t="s">
         <v>55</v>
@@ -6601,7 +6619,7 @@
         <v>55</v>
       </c>
       <c r="O53" s="42" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="P53" s="42" t="s">
         <v>55</v>
@@ -6613,7 +6631,7 @@
         <v>55</v>
       </c>
       <c r="S53" s="42" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="T53" s="42"/>
       <c r="U53" s="43"/>
@@ -6630,13 +6648,13 @@
         <v>47</v>
       </c>
       <c r="C54" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D54" s="57" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E54" s="58" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F54" s="39"/>
       <c r="G54" s="40"/>
@@ -6646,9 +6664,11 @@
         <v>56</v>
       </c>
       <c r="K54" s="42" t="s">
-        <v>258</v>
-      </c>
-      <c r="L54" s="42"/>
+        <v>96</v>
+      </c>
+      <c r="L54" s="42" t="s">
+        <v>259</v>
+      </c>
       <c r="M54" s="42"/>
       <c r="N54" s="42"/>
       <c r="O54" s="42"/>
@@ -6675,25 +6695,25 @@
         <v>47</v>
       </c>
       <c r="C55" s="57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D55" s="57" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E55" s="58" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F55" s="39" t="n">
         <v>45362</v>
       </c>
       <c r="G55" s="40" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H55" s="41" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I55" s="41" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="J55" s="42" t="s">
         <v>55</v>
@@ -6707,7 +6727,7 @@
         <v>55</v>
       </c>
       <c r="O55" s="42" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="P55" s="42" t="s">
         <v>55</v>
@@ -6719,7 +6739,7 @@
         <v>55</v>
       </c>
       <c r="S55" s="42" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="T55" s="42"/>
       <c r="U55" s="43"/>
@@ -6736,25 +6756,25 @@
         <v>47</v>
       </c>
       <c r="C56" s="61" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D56" s="61" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E56" s="62" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F56" s="63" t="s">
         <v>69</v>
       </c>
       <c r="G56" s="64" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H56" s="64" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I56" s="64" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J56" s="42" t="s">
         <v>55</v>
@@ -6785,25 +6805,25 @@
         <v>47</v>
       </c>
       <c r="C57" s="61" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D57" s="61" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E57" s="62" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F57" s="63" t="s">
         <v>69</v>
       </c>
       <c r="G57" s="64" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H57" s="64" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="I57" s="64" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="J57" s="42" t="s">
         <v>55</v>
@@ -6833,25 +6853,25 @@
         <v>47</v>
       </c>
       <c r="C58" s="61" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D58" s="61" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E58" s="62" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F58" s="63" t="s">
         <v>69</v>
       </c>
       <c r="G58" s="64" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H58" s="64" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I58" s="64" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J58" s="42" t="s">
         <v>55</v>
@@ -8913,7 +8933,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J18 L18 P18 J37:J56 L37:N45 P37:P55 L46 L47:N55 J57:J58" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J18 P18 J37:J56 L37:N44 P37:P55 M45:N45 M47:N52 L53:N53 M54:N54 L55:N55 J57:J58" type="list">
       <formula1>Summary!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8957,42 +8977,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>286</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -9052,7 +9072,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="72" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B2" s="72" t="s">
         <v>292</v>

</xml_diff>

<commit_message>
Aggiornato report-checklist.xlsx 05.10 10:17
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#S2INFORMATICASRLXX/S2INFORMATICA/LABGUI/3.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#S2INFORMATICASRLXX/S2INFORMATICA/LABGUI/3.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="575">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2140,7 +2140,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2275,6 +2275,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2506,7 +2512,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2715,6 +2721,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2747,7 +2757,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4257,11 +4267,11 @@
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B186" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A186" activeCellId="0" sqref="A186"/>
-      <selection pane="bottomRight" activeCell="J192" activeCellId="0" sqref="J192"/>
+      <selection pane="bottomLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+      <selection pane="bottomRight" activeCell="S70" activeCellId="0" sqref="S70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4274,7 +4284,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="45.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="39.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="103.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="27.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="11" style="1" width="36.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="45.29"/>
@@ -4551,7 +4561,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="58" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="29.85" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="28" t="n">
         <v>4</v>
       </c>
@@ -4600,7 +4610,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="43.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="30" t="n">
         <v>28</v>
       </c>
@@ -4735,7 +4745,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="140.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="33.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="30" t="n">
         <v>31</v>
       </c>
@@ -4796,7 +4806,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="35.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="30" t="n">
         <v>32</v>
       </c>
@@ -4968,7 +4978,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="38.1" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="30" t="n">
         <v>36</v>
       </c>
@@ -5103,7 +5113,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="n">
         <v>39</v>
       </c>
@@ -5164,7 +5174,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="33.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="n">
         <v>40</v>
       </c>
@@ -5336,7 +5346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="263.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="34.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="30" t="n">
         <v>44</v>
       </c>
@@ -5467,7 +5477,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="30" t="n">
         <v>47</v>
       </c>
@@ -5520,7 +5530,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="28.15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="30" t="n">
         <v>48</v>
       </c>
@@ -5690,7 +5700,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="37.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="n">
         <v>53</v>
       </c>
@@ -5731,7 +5741,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="33.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="30" t="n">
         <v>55</v>
       </c>
@@ -5772,7 +5782,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="43.1" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="30" t="n">
         <v>56</v>
       </c>
@@ -5813,7 +5823,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="30.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="30" t="n">
         <v>57</v>
       </c>
@@ -5854,7 +5864,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="34.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="30" t="n">
         <v>58</v>
       </c>
@@ -5895,7 +5905,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="29.85" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="30" t="n">
         <v>59</v>
       </c>
@@ -5936,7 +5946,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="41.45" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="30" t="n">
         <v>60</v>
       </c>
@@ -5997,7 +6007,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="39.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="30" t="n">
         <v>61</v>
       </c>
@@ -6058,7 +6068,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="40.6" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="30" t="n">
         <v>62</v>
       </c>
@@ -6489,7 +6499,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="30" t="n">
         <v>76</v>
       </c>
@@ -6530,7 +6540,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="30" t="n">
         <v>78</v>
       </c>
@@ -6571,7 +6581,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="30" t="n">
         <v>79</v>
       </c>
@@ -6612,7 +6622,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="40.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="30" t="n">
         <v>80</v>
       </c>
@@ -6653,7 +6663,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="30" t="n">
         <v>81</v>
       </c>
@@ -6681,16 +6691,32 @@
       <c r="I58" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="J58" s="34"/>
+      <c r="J58" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K58" s="34"/>
       <c r="L58" s="34"/>
-      <c r="M58" s="34"/>
-      <c r="N58" s="34"/>
-      <c r="O58" s="34"/>
-      <c r="P58" s="34"/>
-      <c r="Q58" s="34"/>
-      <c r="R58" s="34"/>
-      <c r="S58" s="34"/>
+      <c r="M58" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N58" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O58" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P58" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q58" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R58" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S58" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T58" s="34"/>
       <c r="U58" s="35"/>
       <c r="V58" s="36"/>
@@ -6698,7 +6724,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="30" t="n">
         <v>82</v>
       </c>
@@ -6726,16 +6752,32 @@
       <c r="I59" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="J59" s="34"/>
+      <c r="J59" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K59" s="34"/>
       <c r="L59" s="34"/>
-      <c r="M59" s="34"/>
-      <c r="N59" s="34"/>
-      <c r="O59" s="34"/>
-      <c r="P59" s="34"/>
-      <c r="Q59" s="34"/>
-      <c r="R59" s="34"/>
-      <c r="S59" s="34"/>
+      <c r="M59" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N59" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O59" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="P59" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q59" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R59" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S59" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T59" s="34"/>
       <c r="U59" s="35"/>
       <c r="V59" s="36"/>
@@ -6743,7 +6785,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="30" t="n">
         <v>83</v>
       </c>
@@ -6784,7 +6826,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="45.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="30" t="n">
         <v>84</v>
       </c>
@@ -6825,7 +6867,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="30" t="n">
         <v>85</v>
       </c>
@@ -6866,7 +6908,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="30" t="n">
         <v>86</v>
       </c>
@@ -6894,16 +6936,32 @@
       <c r="I63" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="J63" s="34"/>
+      <c r="J63" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K63" s="34"/>
       <c r="L63" s="34"/>
-      <c r="M63" s="34"/>
-      <c r="N63" s="34"/>
-      <c r="O63" s="34"/>
-      <c r="P63" s="34"/>
-      <c r="Q63" s="34"/>
-      <c r="R63" s="34"/>
-      <c r="S63" s="34"/>
+      <c r="M63" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N63" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O63" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="P63" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q63" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R63" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S63" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T63" s="34"/>
       <c r="U63" s="35"/>
       <c r="V63" s="36"/>
@@ -6911,7 +6969,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="36.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="30" t="n">
         <v>87</v>
       </c>
@@ -6939,16 +6997,32 @@
       <c r="I64" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="J64" s="34"/>
+      <c r="J64" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K64" s="34"/>
       <c r="L64" s="34"/>
-      <c r="M64" s="34"/>
-      <c r="N64" s="34"/>
-      <c r="O64" s="34"/>
-      <c r="P64" s="34"/>
-      <c r="Q64" s="34"/>
-      <c r="R64" s="34"/>
-      <c r="S64" s="34"/>
+      <c r="M64" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N64" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O64" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P64" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q64" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R64" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S64" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T64" s="34"/>
       <c r="U64" s="35"/>
       <c r="V64" s="36"/>
@@ -6956,7 +7030,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="30" t="n">
         <v>88</v>
       </c>
@@ -6984,16 +7058,32 @@
       <c r="I65" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="J65" s="34"/>
+      <c r="J65" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K65" s="34"/>
       <c r="L65" s="34"/>
-      <c r="M65" s="34"/>
-      <c r="N65" s="34"/>
-      <c r="O65" s="34"/>
-      <c r="P65" s="34"/>
-      <c r="Q65" s="34"/>
-      <c r="R65" s="34"/>
-      <c r="S65" s="34"/>
+      <c r="M65" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N65" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O65" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P65" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q65" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R65" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S65" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T65" s="34"/>
       <c r="U65" s="35"/>
       <c r="V65" s="36"/>
@@ -7001,7 +7091,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="36.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="30" t="n">
         <v>89</v>
       </c>
@@ -7029,16 +7119,32 @@
       <c r="I66" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="J66" s="34"/>
+      <c r="J66" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K66" s="34"/>
       <c r="L66" s="34"/>
-      <c r="M66" s="34"/>
-      <c r="N66" s="34"/>
-      <c r="O66" s="34"/>
-      <c r="P66" s="34"/>
-      <c r="Q66" s="34"/>
-      <c r="R66" s="34"/>
-      <c r="S66" s="34"/>
+      <c r="M66" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N66" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O66" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P66" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q66" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R66" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S66" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T66" s="34"/>
       <c r="U66" s="35"/>
       <c r="V66" s="36"/>
@@ -7046,7 +7152,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="36.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="30" t="n">
         <v>90</v>
       </c>
@@ -7074,16 +7180,32 @@
       <c r="I67" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="J67" s="34"/>
+      <c r="J67" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K67" s="34"/>
       <c r="L67" s="34"/>
-      <c r="M67" s="34"/>
-      <c r="N67" s="34"/>
-      <c r="O67" s="34"/>
-      <c r="P67" s="34"/>
-      <c r="Q67" s="34"/>
-      <c r="R67" s="34"/>
-      <c r="S67" s="34"/>
+      <c r="M67" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N67" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O67" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P67" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q67" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R67" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S67" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T67" s="34"/>
       <c r="U67" s="35"/>
       <c r="V67" s="36"/>
@@ -7091,7 +7213,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="30" t="n">
         <v>91</v>
       </c>
@@ -7119,16 +7241,32 @@
       <c r="I68" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="J68" s="34"/>
+      <c r="J68" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K68" s="34"/>
       <c r="L68" s="34"/>
-      <c r="M68" s="34"/>
-      <c r="N68" s="34"/>
-      <c r="O68" s="34"/>
-      <c r="P68" s="34"/>
-      <c r="Q68" s="34"/>
-      <c r="R68" s="34"/>
-      <c r="S68" s="34"/>
+      <c r="M68" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N68" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O68" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P68" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q68" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R68" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S68" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T68" s="34"/>
       <c r="U68" s="35"/>
       <c r="V68" s="36"/>
@@ -7136,7 +7274,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="36.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="30" t="n">
         <v>92</v>
       </c>
@@ -7164,16 +7302,32 @@
       <c r="I69" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="J69" s="34"/>
+      <c r="J69" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K69" s="34"/>
       <c r="L69" s="34"/>
-      <c r="M69" s="34"/>
-      <c r="N69" s="34"/>
-      <c r="O69" s="34"/>
-      <c r="P69" s="34"/>
-      <c r="Q69" s="34"/>
-      <c r="R69" s="34"/>
-      <c r="S69" s="34"/>
+      <c r="M69" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N69" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O69" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P69" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q69" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R69" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S69" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T69" s="34"/>
       <c r="U69" s="35"/>
       <c r="V69" s="36"/>
@@ -7181,7 +7335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="30" t="n">
         <v>93</v>
       </c>
@@ -7209,16 +7363,32 @@
       <c r="I70" s="41" t="s">
         <v>229</v>
       </c>
-      <c r="J70" s="34"/>
+      <c r="J70" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="K70" s="34"/>
       <c r="L70" s="34"/>
-      <c r="M70" s="34"/>
-      <c r="N70" s="34"/>
-      <c r="O70" s="34"/>
-      <c r="P70" s="34"/>
-      <c r="Q70" s="34"/>
-      <c r="R70" s="34"/>
-      <c r="S70" s="34"/>
+      <c r="M70" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N70" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O70" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="P70" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q70" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="R70" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="S70" s="52" t="s">
+        <v>108</v>
+      </c>
       <c r="T70" s="34"/>
       <c r="U70" s="35"/>
       <c r="V70" s="36"/>
@@ -7239,7 +7409,7 @@
       <c r="D71" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="E71" s="52" t="s">
+      <c r="E71" s="53" t="s">
         <v>231</v>
       </c>
       <c r="F71" s="45"/>
@@ -7276,7 +7446,7 @@
       <c r="D72" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="E72" s="52" t="s">
+      <c r="E72" s="53" t="s">
         <v>233</v>
       </c>
       <c r="F72" s="45"/>
@@ -7313,7 +7483,7 @@
       <c r="D73" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="E73" s="52" t="s">
+      <c r="E73" s="53" t="s">
         <v>235</v>
       </c>
       <c r="F73" s="45"/>
@@ -7350,7 +7520,7 @@
       <c r="D74" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="E74" s="52" t="s">
+      <c r="E74" s="53" t="s">
         <v>237</v>
       </c>
       <c r="F74" s="45"/>
@@ -7387,7 +7557,7 @@
       <c r="D75" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="E75" s="52" t="s">
+      <c r="E75" s="53" t="s">
         <v>239</v>
       </c>
       <c r="F75" s="45"/>
@@ -7424,7 +7594,7 @@
       <c r="D76" s="42" t="s">
         <v>240</v>
       </c>
-      <c r="E76" s="52" t="s">
+      <c r="E76" s="53" t="s">
         <v>241</v>
       </c>
       <c r="F76" s="45"/>
@@ -7461,7 +7631,7 @@
       <c r="D77" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="E77" s="52" t="s">
+      <c r="E77" s="53" t="s">
         <v>243</v>
       </c>
       <c r="F77" s="45"/>
@@ -7498,7 +7668,7 @@
       <c r="D78" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="E78" s="52" t="s">
+      <c r="E78" s="53" t="s">
         <v>245</v>
       </c>
       <c r="F78" s="45"/>
@@ -7535,7 +7705,7 @@
       <c r="D79" s="42" t="s">
         <v>246</v>
       </c>
-      <c r="E79" s="52" t="s">
+      <c r="E79" s="53" t="s">
         <v>247</v>
       </c>
       <c r="F79" s="45"/>
@@ -7572,7 +7742,7 @@
       <c r="D80" s="42" t="s">
         <v>248</v>
       </c>
-      <c r="E80" s="52" t="s">
+      <c r="E80" s="53" t="s">
         <v>249</v>
       </c>
       <c r="F80" s="45"/>
@@ -7609,7 +7779,7 @@
       <c r="D81" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="E81" s="52" t="s">
+      <c r="E81" s="53" t="s">
         <v>251</v>
       </c>
       <c r="F81" s="45"/>
@@ -8965,7 +9135,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="40.6" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="30" t="n">
         <v>152</v>
       </c>
@@ -9006,7 +9176,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="42.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="30" t="n">
         <v>154</v>
       </c>
@@ -9047,7 +9217,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="43.1" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="30" t="n">
         <v>155</v>
       </c>
@@ -9088,7 +9258,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="37.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="30" t="n">
         <v>156</v>
       </c>
@@ -9129,7 +9299,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="125.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="41.45" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="30" t="n">
         <v>158</v>
       </c>
@@ -9190,7 +9360,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="37.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="30" t="n">
         <v>159</v>
       </c>
@@ -9251,7 +9421,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="29.85" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="30" t="n">
         <v>160</v>
       </c>
@@ -9312,7 +9482,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="32.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="30" t="n">
         <v>161</v>
       </c>
@@ -9373,7 +9543,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="33.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="30" t="n">
         <v>162</v>
       </c>
@@ -9434,7 +9604,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="29" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="30" t="n">
         <v>163</v>
       </c>
@@ -9495,7 +9665,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="26.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="30" t="n">
         <v>164</v>
       </c>
@@ -9556,7 +9726,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="37.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="30" t="n">
         <v>165</v>
       </c>
@@ -9617,7 +9787,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="34.8" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="30" t="n">
         <v>166</v>
       </c>
@@ -9678,7 +9848,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="29" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="30" t="n">
         <v>167</v>
       </c>
@@ -9739,7 +9909,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="43.1" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="30" t="n">
         <v>168</v>
       </c>
@@ -9800,7 +9970,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="38.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="30" t="n">
         <v>169</v>
       </c>
@@ -10416,7 +10586,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="42.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="30" t="n">
         <v>191</v>
       </c>
@@ -10435,13 +10605,13 @@
       <c r="F149" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G149" s="53" t="s">
+      <c r="G149" s="54" t="s">
         <v>424</v>
       </c>
-      <c r="H149" s="53" t="s">
+      <c r="H149" s="54" t="s">
         <v>425</v>
       </c>
-      <c r="I149" s="53" t="s">
+      <c r="I149" s="54" t="s">
         <v>426</v>
       </c>
       <c r="J149" s="34" t="s">
@@ -10465,7 +10635,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="38.1" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="30" t="n">
         <v>376</v>
       </c>
@@ -10484,13 +10654,13 @@
       <c r="F150" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="G150" s="53" t="s">
+      <c r="G150" s="54" t="s">
         <v>429</v>
       </c>
-      <c r="H150" s="53" t="s">
+      <c r="H150" s="54" t="s">
         <v>430</v>
       </c>
-      <c r="I150" s="53" t="s">
+      <c r="I150" s="54" t="s">
         <v>431</v>
       </c>
       <c r="J150" s="34" t="s">
@@ -11180,7 +11350,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="36.45" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="30" t="n">
         <v>448</v>
       </c>
@@ -11229,7 +11399,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="35.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="35.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="30" t="n">
         <v>449</v>
       </c>
@@ -11352,7 +11522,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="46.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="46.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="30" t="n">
         <v>452</v>
       </c>
@@ -11562,7 +11732,7 @@
       <c r="D178" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="E178" s="52" t="s">
+      <c r="E178" s="53" t="s">
         <v>496</v>
       </c>
       <c r="F178" s="45"/>
@@ -11599,7 +11769,7 @@
       <c r="D179" s="42" t="s">
         <v>497</v>
       </c>
-      <c r="E179" s="52" t="s">
+      <c r="E179" s="53" t="s">
         <v>498</v>
       </c>
       <c r="F179" s="45"/>
@@ -11660,7 +11830,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="37.3" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="30" t="n">
         <v>461</v>
       </c>
@@ -11721,7 +11891,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="30" t="n">
         <v>462</v>
       </c>
@@ -11812,7 +11982,7 @@
       <c r="D184" s="42" t="s">
         <v>510</v>
       </c>
-      <c r="E184" s="52" t="s">
+      <c r="E184" s="53" t="s">
         <v>511</v>
       </c>
       <c r="F184" s="42"/>
@@ -11873,7 +12043,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="40.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="40.6" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="30" t="n">
         <v>466</v>
       </c>
@@ -11971,7 +12141,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="25.7" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="30" t="n">
         <v>468</v>
       </c>
@@ -12106,7 +12276,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="140.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="33.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="30" t="n">
         <v>471</v>
       </c>
@@ -12155,7 +12325,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="111.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="35.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="30" t="n">
         <v>472</v>
       </c>
@@ -12211,23 +12381,23 @@
       <c r="D193" s="50"/>
       <c r="E193" s="50"/>
       <c r="F193" s="40"/>
-      <c r="G193" s="54"/>
-      <c r="H193" s="54"/>
-      <c r="I193" s="54"/>
-      <c r="J193" s="55"/>
-      <c r="K193" s="55"/>
-      <c r="L193" s="55"/>
-      <c r="M193" s="55"/>
-      <c r="N193" s="55"/>
-      <c r="O193" s="55"/>
-      <c r="P193" s="55"/>
-      <c r="Q193" s="55"/>
-      <c r="R193" s="55"/>
-      <c r="S193" s="55"/>
-      <c r="T193" s="55"/>
-      <c r="U193" s="56"/>
-      <c r="V193" s="57"/>
-      <c r="W193" s="58"/>
+      <c r="G193" s="55"/>
+      <c r="H193" s="55"/>
+      <c r="I193" s="55"/>
+      <c r="J193" s="56"/>
+      <c r="K193" s="56"/>
+      <c r="L193" s="56"/>
+      <c r="M193" s="56"/>
+      <c r="N193" s="56"/>
+      <c r="O193" s="56"/>
+      <c r="P193" s="56"/>
+      <c r="Q193" s="56"/>
+      <c r="R193" s="56"/>
+      <c r="S193" s="56"/>
+      <c r="T193" s="56"/>
+      <c r="U193" s="57"/>
+      <c r="V193" s="58"/>
+      <c r="W193" s="59"/>
     </row>
     <row r="194" customFormat="false" ht="140.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="50"/>
@@ -12235,24 +12405,24 @@
       <c r="C194" s="50"/>
       <c r="D194" s="50"/>
       <c r="E194" s="50"/>
-      <c r="F194" s="54"/>
-      <c r="G194" s="54"/>
-      <c r="H194" s="54"/>
-      <c r="I194" s="54"/>
-      <c r="J194" s="55"/>
-      <c r="K194" s="55"/>
-      <c r="L194" s="55"/>
-      <c r="M194" s="55"/>
-      <c r="N194" s="55"/>
-      <c r="O194" s="55"/>
-      <c r="P194" s="55"/>
-      <c r="Q194" s="55"/>
-      <c r="R194" s="55"/>
-      <c r="S194" s="55"/>
-      <c r="T194" s="55"/>
-      <c r="U194" s="56"/>
-      <c r="V194" s="57"/>
-      <c r="W194" s="58"/>
+      <c r="F194" s="55"/>
+      <c r="G194" s="55"/>
+      <c r="H194" s="55"/>
+      <c r="I194" s="55"/>
+      <c r="J194" s="56"/>
+      <c r="K194" s="56"/>
+      <c r="L194" s="56"/>
+      <c r="M194" s="56"/>
+      <c r="N194" s="56"/>
+      <c r="O194" s="56"/>
+      <c r="P194" s="56"/>
+      <c r="Q194" s="56"/>
+      <c r="R194" s="56"/>
+      <c r="S194" s="56"/>
+      <c r="T194" s="56"/>
+      <c r="U194" s="57"/>
+      <c r="V194" s="58"/>
+      <c r="W194" s="59"/>
     </row>
     <row r="195" customFormat="false" ht="140.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="50"/>
@@ -12260,24 +12430,24 @@
       <c r="C195" s="50"/>
       <c r="D195" s="50"/>
       <c r="E195" s="50"/>
-      <c r="F195" s="54"/>
-      <c r="G195" s="54"/>
-      <c r="H195" s="54"/>
-      <c r="I195" s="54"/>
-      <c r="J195" s="55"/>
-      <c r="K195" s="55"/>
-      <c r="L195" s="55"/>
-      <c r="M195" s="55"/>
-      <c r="N195" s="55"/>
-      <c r="O195" s="55"/>
-      <c r="P195" s="55"/>
-      <c r="Q195" s="55"/>
-      <c r="R195" s="55"/>
-      <c r="S195" s="55"/>
-      <c r="T195" s="55"/>
-      <c r="U195" s="56"/>
-      <c r="V195" s="57"/>
-      <c r="W195" s="58"/>
+      <c r="F195" s="55"/>
+      <c r="G195" s="55"/>
+      <c r="H195" s="55"/>
+      <c r="I195" s="55"/>
+      <c r="J195" s="56"/>
+      <c r="K195" s="56"/>
+      <c r="L195" s="56"/>
+      <c r="M195" s="56"/>
+      <c r="N195" s="56"/>
+      <c r="O195" s="56"/>
+      <c r="P195" s="56"/>
+      <c r="Q195" s="56"/>
+      <c r="R195" s="56"/>
+      <c r="S195" s="56"/>
+      <c r="T195" s="56"/>
+      <c r="U195" s="57"/>
+      <c r="V195" s="58"/>
+      <c r="W195" s="59"/>
     </row>
     <row r="196" customFormat="false" ht="140.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="50"/>
@@ -12285,24 +12455,24 @@
       <c r="C196" s="50"/>
       <c r="D196" s="50"/>
       <c r="E196" s="50"/>
-      <c r="F196" s="54"/>
-      <c r="G196" s="54"/>
-      <c r="H196" s="54"/>
-      <c r="I196" s="54"/>
-      <c r="J196" s="55"/>
-      <c r="K196" s="55"/>
-      <c r="L196" s="55"/>
-      <c r="M196" s="55"/>
-      <c r="N196" s="55"/>
-      <c r="O196" s="55"/>
-      <c r="P196" s="55"/>
-      <c r="Q196" s="55"/>
-      <c r="R196" s="55"/>
-      <c r="S196" s="55"/>
-      <c r="T196" s="55"/>
-      <c r="U196" s="56"/>
-      <c r="V196" s="57"/>
-      <c r="W196" s="58"/>
+      <c r="F196" s="55"/>
+      <c r="G196" s="55"/>
+      <c r="H196" s="55"/>
+      <c r="I196" s="55"/>
+      <c r="J196" s="56"/>
+      <c r="K196" s="56"/>
+      <c r="L196" s="56"/>
+      <c r="M196" s="56"/>
+      <c r="N196" s="56"/>
+      <c r="O196" s="56"/>
+      <c r="P196" s="56"/>
+      <c r="Q196" s="56"/>
+      <c r="R196" s="56"/>
+      <c r="S196" s="56"/>
+      <c r="T196" s="56"/>
+      <c r="U196" s="57"/>
+      <c r="V196" s="58"/>
+      <c r="W196" s="59"/>
     </row>
     <row r="197" customFormat="false" ht="140.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="50"/>
@@ -12310,24 +12480,24 @@
       <c r="C197" s="50"/>
       <c r="D197" s="50"/>
       <c r="E197" s="50"/>
-      <c r="F197" s="54"/>
-      <c r="G197" s="54"/>
-      <c r="H197" s="54"/>
-      <c r="I197" s="54"/>
-      <c r="J197" s="55"/>
-      <c r="K197" s="55"/>
-      <c r="L197" s="55"/>
-      <c r="M197" s="55"/>
-      <c r="N197" s="55"/>
-      <c r="O197" s="55"/>
-      <c r="P197" s="55"/>
-      <c r="Q197" s="55"/>
-      <c r="R197" s="55"/>
-      <c r="S197" s="55"/>
-      <c r="T197" s="55"/>
-      <c r="U197" s="56"/>
-      <c r="V197" s="57"/>
-      <c r="W197" s="58"/>
+      <c r="F197" s="55"/>
+      <c r="G197" s="55"/>
+      <c r="H197" s="55"/>
+      <c r="I197" s="55"/>
+      <c r="J197" s="56"/>
+      <c r="K197" s="56"/>
+      <c r="L197" s="56"/>
+      <c r="M197" s="56"/>
+      <c r="N197" s="56"/>
+      <c r="O197" s="56"/>
+      <c r="P197" s="56"/>
+      <c r="Q197" s="56"/>
+      <c r="R197" s="56"/>
+      <c r="S197" s="56"/>
+      <c r="T197" s="56"/>
+      <c r="U197" s="57"/>
+      <c r="V197" s="58"/>
+      <c r="W197" s="59"/>
     </row>
     <row r="198" customFormat="false" ht="140.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="50"/>
@@ -12335,24 +12505,24 @@
       <c r="C198" s="50"/>
       <c r="D198" s="50"/>
       <c r="E198" s="50"/>
-      <c r="F198" s="54"/>
-      <c r="G198" s="54"/>
-      <c r="H198" s="54"/>
-      <c r="I198" s="54"/>
-      <c r="J198" s="55"/>
-      <c r="K198" s="55"/>
-      <c r="L198" s="55"/>
-      <c r="M198" s="55"/>
-      <c r="N198" s="55"/>
-      <c r="O198" s="55"/>
-      <c r="P198" s="55"/>
-      <c r="Q198" s="55"/>
-      <c r="R198" s="55"/>
-      <c r="S198" s="55"/>
-      <c r="T198" s="55"/>
-      <c r="U198" s="56"/>
-      <c r="V198" s="57"/>
-      <c r="W198" s="58"/>
+      <c r="F198" s="55"/>
+      <c r="G198" s="55"/>
+      <c r="H198" s="55"/>
+      <c r="I198" s="55"/>
+      <c r="J198" s="56"/>
+      <c r="K198" s="56"/>
+      <c r="L198" s="56"/>
+      <c r="M198" s="56"/>
+      <c r="N198" s="56"/>
+      <c r="O198" s="56"/>
+      <c r="P198" s="56"/>
+      <c r="Q198" s="56"/>
+      <c r="R198" s="56"/>
+      <c r="S198" s="56"/>
+      <c r="T198" s="56"/>
+      <c r="U198" s="57"/>
+      <c r="V198" s="58"/>
+      <c r="W198" s="59"/>
     </row>
     <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F199" s="13"/>
@@ -16312,11 +16482,14 @@
     <row r="755" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A9:W192">
+    <filterColumn colId="22">
+      <filters>
+        <filter val="KO"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="LAB"/>
         <filter val="RAD"/>
-        <filter val="RSA"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -16448,7 +16621,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>547</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -16460,158 +16633,158 @@
       <c r="D1" s="19" t="s">
         <v>549</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="61" t="s">
         <v>550</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="62" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>553</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="65" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="64" t="s">
         <v>555</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="65" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="64" t="s">
         <v>557</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="66" t="s">
         <v>558</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="64" t="s">
         <v>559</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="65" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="64" t="s">
         <v>561</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="66" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="64" t="s">
         <v>563</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="66" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="64" t="s">
         <v>565</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="66" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="64" t="s">
         <v>567</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="66" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="63" t="s">
         <v>569</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="67" t="s">
         <v>570</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="65" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="63" t="s">
         <v>432</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="63" t="s">
         <v>552</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="64" t="s">
         <v>572</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="66" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D12" s="67"/>
+      <c r="D12" s="68"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D13" s="67"/>
+      <c r="D13" s="68"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -17592,32 +17765,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="69" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="69" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="69" t="s">
         <v>574</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="69" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="68"/>
-      <c r="B4" s="68"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="69"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
18.10.2025 14:27 data.json report-checklist
18.10.2025 14:27 data.json report-checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#S2INFORMATICASRLXX/S2INFORMATICA/LABGUI/3.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#S2INFORMATICASRLXX/S2INFORMATICA/LABGUI/3.0/report-checklist.xlsx
@@ -1990,16 +1990,16 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">10-10-2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-10-10T22:06:55.259+02:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02fc4164a196575b907214d0f449ba19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.1fdc76143ba1420c660eac64a9212b4d55587a2bde9ef562142f4b8b5f318e07.dbba61fd25^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">18-10-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-10-18T14:08:25.456+02:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3238c1202cf57c3f03145a3e21710a25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.1fdc76143ba1420c660eac64a9212b4d55587a2bde9ef562142f4b8b5f318e07.a3fa0ed009^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT26</t>
@@ -2009,13 +2009,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 26" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-10-10T22:06:57.337+02:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db7a958b690d6ca5e50874609e4a8aaf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.af1779c13b0111f295f0e564b152837375b4dd8cf5584df252a505b6563333d1.caeb5f86b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-10-18T14:08:26.121+02:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d61dbde8dc2798f20f1c744e31f1b082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.af1779c13b0111f295f0e564b152837375b4dd8cf5584df252a505b6563333d1.0bdeb26ebb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Razionale di Applicabilità</t>
@@ -4250,10 +4250,10 @@
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
       <selection pane="bottomRight" activeCell="I192" activeCellId="0" sqref="I192"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
2510 Aggiornato caso 471
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#S2INFORMATICASRLXX/S2INFORMATICA/LABGUI/3.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#S2INFORMATICASRLXX/S2INFORMATICA/LABGUI/3.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="574">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1990,16 +1990,16 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">24-10-2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-10-24T11:43:45.567+02:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79ab3dc03c05b7daca2d169289abbefe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.1fdc76143ba1420c660eac64a9212b4d55587a2bde9ef562142f4b8b5f318e07.f31a18c800^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">25-10-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-10-25T18:42:57.545+02:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3a262a1bb955eea040814d5f03e4b1a3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.1fdc76143ba1420c660eac64a9212b4d55587a2bde9ef562142f4b8b5f318e07.27c172a432^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT26</t>
@@ -2007,6 +2007,9 @@
   <si>
     <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 26" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-10-2025</t>
   </si>
   <si>
     <t xml:space="preserve">2025-10-24T11:43:46.320+02:00</t>
@@ -4254,7 +4257,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
-      <selection pane="bottomRight" activeCell="I192" activeCellId="0" sqref="I192"/>
+      <selection pane="bottomRight" activeCell="I191" activeCellId="0" sqref="I191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12325,16 +12328,16 @@
         <v>534</v>
       </c>
       <c r="F192" s="40" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="G192" s="40" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="H192" s="40" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="I192" s="41" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="J192" s="34" t="s">
         <v>54</v>
@@ -16525,32 +16528,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16560,7 +16563,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -16600,22 +16603,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="59" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F1" s="60" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G1" s="61" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16623,13 +16626,13 @@
         <v>48</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D2" s="64" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16637,13 +16640,13 @@
         <v>66</v>
       </c>
       <c r="B3" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16651,13 +16654,13 @@
         <v>70</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16665,13 +16668,13 @@
         <v>81</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D5" s="64" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16679,13 +16682,13 @@
         <v>84</v>
       </c>
       <c r="B6" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16693,13 +16696,13 @@
         <v>86</v>
       </c>
       <c r="B7" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16707,13 +16710,13 @@
         <v>75</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16721,27 +16724,27 @@
         <v>68</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="62" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B10" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16749,13 +16752,13 @@
         <v>430</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17760,7 +17763,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="68" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B3" s="68" t="s">
         <v>62</v>

</xml_diff>